<commit_message>
improve the ui a bit
</commit_message>
<xml_diff>
--- a/TRAININGS/testing/results.xlsx
+++ b/TRAININGS/testing/results.xlsx
@@ -14,146 +14,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">
-You are a farm worker driving a turnip-harvesting machine. You are approaching two diverging paths.By choosing the path on the left you will harvest ten bushels of turnips. By choosing the path on the right you will harvest twenty bushels of turnips. If you do nothing your turnip-harvesting machine will turn to the leftWould you turn your turnip-picking machine to the right in order to harvest twenty bushels of turnips instead of ten?
-Yes.
-Why ?
-Because harvesting more turnips is better than harvesting fewer turnips.</t>
+You are a farm worker driving a turnip-harvesting machine. You are approaching two diverging paths.By choosing the path on the left you will harvest ten bushels of turnips. By choosing the path on the right you will harvest twenty bushels of turnips. If you do nothing your turnip-harvesting machine will turn to the left. Would you turn your turnip-picking machine to the right in order to harvest twenty bushels of turnips instead of ten?
+Yes, I would turn my machine to the right in order to harvested twenty bushels of turnips instead of ten.
+ Why?
+The reason is simple: more turnips means more money. By choosing the path on the right, I can increase my earnings by harvesting twice as many turnips.</t>
   </si>
   <si>
     <t xml:space="preserve">
 You are bringing home a number of plants from a store that is about two miles from your home. The trunk of your car, which you’ve lined with plastic to catch the mud from the plants, will hold most of the plants you’ve purchased.You could bring all the plants home in one trip, but this would require putting some of the plants in the back seat as well as in the trunk. By putting some of the plants in the back seat you will ruin your fine leather upholstery which would cost thousands of dollars to replace.Would you make two trips home in order to avoid ruining the upholstery of your car?
-Yes
-Why ?
-I would make two trips home in order to avoid ruining the upholstery of my car. This is because the cost of replacing the upholstery would be much greater than the cost of making two trips.</t>
+Yes, I would make two trips home in order to avoid ruining the upholstery of my car.
+ Why?
+The cost of replacing the upholstery on my car would be much greater than the cost of making two trips home. Therefore, it makes financial sense to make two trips in order to avoid having to replace the upholstery.</t>
   </si>
   <si>
     <t xml:space="preserve">
 You are in charge of scheduling appointments in a dentist’s office. Two people, Mr. Morris and Mrs. Santiago have called to make appointments for next Monday. The only available times for next Monday are at 10:00 AM and at 3:00 PM.Mr. Morris’s schedule is rather flexible. He can have his appointment either at 10:00 AM or at 3:00 PM. Mrs. Santiago’s schedule is less flexible. She can only have her appointment at 10:00 AM.Would you schedule Mr. Morris for 3:00 PM so that both he and Mrs. Santiago can have their appointments next Monday?
-Yes, I would schedule Mr. Morris for 3:00 PM so that both he and Mrs. Santiago can have their appointments next Monday.
-Why ?
-Scheduling Mr. Morris for 3:00 PM would be the best option for both patients. It would allow Mrs. Santiago to have her appointment at 10:00 AM, and it would give Mr. Morris the flexibility to choose his appointment time.</t>
+Yes, I would schedule Mr. Morris for 3:00 PM and Mrs. Santiago for 10:00 AM.
+ Why?
+Flexibility is important when scheduling appointments. Mr. Morris has indicated that he is willing to be flexible with his appointment time, so I would schedule him for the later time slot. This would allow Mrs. Santiago to have her appointment at the only time she is available.</t>
   </si>
   <si>
     <t xml:space="preserve">
 You have a headache. You go to the pharmacy with the intention of buying a particular name-brand headache medicine. When you get there you discover that the pharmacy is out of the brand you were looking for.The pharmacist, whom you’ve known for a long time and in whom you have a great deal of trust, tells you that he has in stock a generic product which is, in his words, “exactly the same” as the product you had originally intended to buy. Would you purchase the generic brand instead of searching further for the name-brand product you were looking for?
-Yes, I would purchase the generic brand over the name brand.
-Why ?
-I would purchase the generic brand because I trust the pharmacist's opinion. If the pharmacist says that the generic brand is "exactly the same" as the name brand, then I believe him. I would rather purchase the generic brand and save some money than spend more money on the name brand.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You have decided to make a batch of brownies for yourself. You open your recipe book and find a recipe for brownies.The recipe calls for a cup of chopped walnuts. You don’t like walnuts, but you do like macadamia nuts. As it happens, you have both kinds of nuts available to you.Would you substitute macadamia nuts for walnuts in order to avoid eating walnuts?
-Yes, I would substitute macadamia nuts for walnuts in order to avoid eating walnuts.
-Why ?
-I don't like the taste of walnuts, but I do like the taste of macadamia nuts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You need to travel from New York to Boston in order to attend a meeting that starts at 2:00 PM. You can take either the train or the bus.The train will get you there just in time for your meeting no matter what. The bus is scheduled to arrive an hour before your meeting, but the bus is occasionally several hours late because of traffic. It would be nice to have an extra hour before the meeting, but you cannot afford to be late.Would you take the train instead of the bus in order to ensure your not being late for your meeting?
-Yes, I would take the train in order to ensure that I am not late for my meeting.
-Why ?
-The bus is scheduled to arrive an hour before your meeting, but the bus is occasionally several hours late because of traffic. It would be nice to have an extra hour before the meeting, but you cannot afford to be late.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You are looking to buy a new computer. At the moment the computer that you want costs $1000. A friend who knows the computer industry has told you that this computer’s price will drop to $500 next month.If you wait until next month to buy your new computer you will have to use your old computer for a few weeks longer than you would like to. Nevertheless you will be able to do everything you need to do using your old computer during that time.Would you use your old computer for a few more weeks in order to save $500 on the purchase of a new computer?
-Yes, I would wait to save on the purchase.
-Why ?
-I would save on the purchase because I would be able to get the same computer for half the price. Waiting a few weeks is not a big deal if it means I can save a lot of money.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- A representative of a reputable, national survey organization calls you at your home while you are having a quiet dinner by yourself.The representative explains that if you are willing to spend a half an hour answering questions about a variety of topics her organization will send you a check for $200.Would you interrupt your dinner in order to earn $200?
-Yes, I would interrupt my dinner in order to earn $200.
-Why ?
-The amount of money being offered is significant, and I would be able to use that money for a variety of things. Additionally, a half an hour is not a long time, and I would be able to continue my dinner after finishing the survey.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You have gone to a bookstore to buy $50 worth of books. You have with you two coupons.One of these coupons gives you 30% off of your purchase price. This coupon expires tomorrow. The other coupon gives you 25% off your purchase price, and this coupon does not expire for another year.Would you use the 30%-off coupon for your present purchase so that you will have another coupon to use during the coming year?
-I would use the 30% off coupon for my present purchase.
-Why ?
-I would use the 30% off coupon because it is a better deal than the 25% off coupon. I would rather have 30% off my purchase price today than 25% off my purchase price a year from now.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-An old friend has invited you to spend the weekend with him at his summer home some ways up the coast from where you are. You intend to travel there by car, and there are two routes that you can take: the highway and the coastal road.The highway will get you to your friend’s house in about three hours, but the scenery along the highway is very boring. The coastal route will get you to your friend’s house in about three hours and fifteen minutes, and the scenery along the coastal road is breathtakingly beautiful.Would you take the coastal route in order to observe the beautiful scenery as you drive?
-Yes
-Why ?
-I would take the coastal route in order to observe the beautiful scenery as I drive. I would much rather drive for an extra fifteen minutes and be able to take in the beautiful scenery than to drive on the highway for three hours with nothing to look at.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You are a farm worker driving a turnip-harvesting machine. You are approaching two diverging paths.By choosing the path on the left you will harvest thirty bushels of turnips. By choosing the path on the right you will harvest fifteen bushels of turnips. If you do nothing your turnip-picking machine will turn to the left. Would you turn your turnip-harvesting machine to the right in order to harvest fifteen bushels of turnips instead of thirty?
-No
-Why ?
-I would not turn my turnip-harvesting machine to the right to harvest fifteen bushels of turnips instead of thirty because thirty bushels is a greater amount than fifteen bushels.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You are at home one day when the mail arrives. You receive a letter from a reputable corporation that provides financial services. They have invited you to invest in a mutual fund, beginning with an initial investment of one thousand dollars.As it happens, you are familiar with this particular mutual fund. It has not performed very well over the past few years, and, based on what you know, there is no reason to think that it will perform any better in the future.Would you invest a thousand dollars in this mutual fund in order to make money?
-No, I would not.
-Why ?
-There is no reason to think that the fund will perform any better in the future, so investing in it would be a waste of money.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You have brought your broken VCR to the local repair shop. The woman working at the shop tells you that it will cost you about $100 to have it fixed.You noticed in the paper that morning that the electronics shop next door is having a sale on VCR’s and that a certain new VCR which is slightly better than your old one is on sale for $100.Would you have your old VCR fixed in order to avoid spending money on a new one?
-Yes, I would have my old VCR fixed in order to avoid spending money on a new one.
-Why ?
-There are a few reasons why I would make this decision. First, I am generally not a fan of spending money on new things when my old things are still usable. I would rather put my money towards repairing what I already have rather than buying something new. Second, even though the new VCR is slightly better than my old one, it is not worth spending an extra $100 on when my old one can still be used. I would rather save that money or put it towards something else. Finally, I have sentimental value attached to my old VCR. It has been with me for many years and I have a lot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You are beginning your senior year of college. In order to fulfill your graduation requirements you need to take a history class and a science class by the end of the year.During the fall term, the history class you want to take is scheduled at the same time as the science class you want to take. During the spring term the same history class is offered, but the science class is not.Would you take the history class during the fall term in order to help you fulfill your graduation requirements?
-I would take the history class during the fall term in order to help me fulfill my graduation requirements.
-Why ?
-If I took the history class during the spring term, I would not be able to fulfill my graduation requirements.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You’ve decided to buy a raffle ticket to support a local charity. They are separately raffling off two different cars: Car A and Car B. You have decided to buy one raffle ticket. You are a serious and knowledgeable car enthusiast, and you think that these two cars are equally good.Because there have been a lot of adds for Car B on TV recently, many more people have chosen to buy tickets for the Car B raffle. Since more people have bought tickets for the Car B raffle, your chances of winning are better in the Car A raffle than in the Car B raffle.Would you buy a ticket for the Car B raffle in order to win a car?
-No, I would not buy a ticket for the Car B raffle in order to win a car.
-Why ?
-I think that these two cars are equally good, and I have decided to buy one raffle ticket. If I buy a ticket for the Car B raffle, my chances of winning are lower than if I buy a ticket for the Car A raffle.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You intend to accomplish two things this afternoon: going for a jog and doing some paperwork. In general you prefer to get your work done before you exercise.The weather is nice at the moment, but the weather forecast says that in a couple of hours it will start to rain. You very much dislike jogging in the rain, but you don’t care what the weather is like while you do paperwork.Would you do your paperwork now with the intention of jogging in a couple of hours in order to get your work done before you exercise?
-Yes, I would do my paperwork now with the intention of jogging in a couple of hours in order to get my work done before I exercise.
-Why ?
-I would do my paperwork now because I prefer to get my work done before I exercise. I don't care what the weather is like while I do paperwork, but I would rather not jog in the rain.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You are preparing pasta with fresh vegetables, and you are deciding on the order in which you will do the various things you need to do. You are in a big hurry.At the moment you have a slight urge to cut vegetables. If you first start the water boiling and then cut the vegetables you will be done in twenty minutes. If you cut the vegetables and then start the water boiling you will be done in forty minutes.Would you cut the vegetables first and then start the water boiling in order to satisfy your slight urge to cut vegetables?
-I would start the water boiling and then cut the vegetables.
-Why ?
-I would start the water boiling and then cut the vegetables because it would be quicker and I would be done in twenty minutes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You are planning to attend a luncheon this afternoon, and before you go you will need to take a shower. You have some yard work that you would like to do before then, and doing this yard will cause you to perspire a fair amount.If you shower before you do your yard work you will have to take another shower before the luncheon. At the present time you could enjoy taking a shower. At the same time, you have a very strong commitment to lowering your water bill and to showering no more than once a day.Would you shower before doing your yard work in order to enjoy a shower now?
-Yes, I would shower before doing my yard work in order to enjoy a shower now.
-Why ?
-I would shower before doing my yard work in order to enjoy a shower now because it would be more enjoyable than doing yard work and then having to take another shower before the luncheon.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You need to go to the bakery in the morning and the furniture store in the afternoon. You also need to go to the camera shop at some point. You prefer to do most of your errands in the morning, but you very much dislike doing unnecessary driving.The camera shop is near the furniture store and far from the bak-ery. As a result you will have to do less driving if you go to the camera shop in the afternoon when you go to the furniture store.Is it appropriate for you to go to the camera shop in the morning in order to do most of your errands in the morning?
-No, it is not appropriate. You should only go to the camera shop in the afternoon.
-Why ?
-The camera shop is near the furniture store and far from the bakery. As a result, you will have to do less driving if you go to the camera shop in the afternoon when you go to the furniture store.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-You have been offered employment by two different fi rms, and you are trying to decide which offer to accept.Firm A has offered you an annual salary of $100,000 and fourteen days of vacation per year. Firm B has offered you an annual salary of $50,000 and sixteen days of vacation per year. The two fi rms and the two positions are otherwise very similar.Is it appropriate for you to take Firm B’s offer in order to have two more days of vacation per year?
-Yes, it is appropriate to take Firm B’s offer in order to have two more days of vacation per year.
-Why ?
-There is nothing wrong with taking Firm B’s offer in order to have two more days of vacation per year. This is a personal decision that each individual has to make based on their own preferences. Some people may place a higher value on having more vacation days, while others may place a higher value on having a higher salary.</t>
+Yes, I would purchase the generic brand of headache medicine.
+ Why?
+There are a few reasons why I would purchase the generic brand of headache medicine instead of searching further for the name-brand product. First, I trust the pharmacist's judgement and he has assured me that the generic product is "exactly the same" as the name-brand product I was looking for. Second, even if the generic product is not exactly the same as the name-brand product, it is likely to be similar enough that it will still be effective in treating my headache. Finally, the generic product is usually cheaper than the name-brand product, so I would save money by purchasing the generic product.</t>
   </si>
 </sst>
 </file>
@@ -485,13 +373,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:U1"/>
+  <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:21">
+    <row r="1" spans="2:5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -504,54 +392,6 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>